<commit_message>
STAI updated Sep 10
</commit_message>
<xml_diff>
--- a/List of Questionnaires.xlsx
+++ b/List of Questionnaires.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yubing/Downloads/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yubing/Desktop/Questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C461BB-54FD-BC42-B814-2139C0C17CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4746DBA-2195-BA4E-A8BF-45399BB9D7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10260" yWindow="500" windowWidth="28040" windowHeight="15580" xr2:uid="{9BF46821-2083-9D45-B470-57895F576DB5}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15580" xr2:uid="{9BF46821-2083-9D45-B470-57895F576DB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -144,12 +144,6 @@
     <t>SCARED-CV</t>
   </si>
   <si>
-    <t>STAI</t>
-  </si>
-  <si>
-    <t>STAI-Y</t>
-  </si>
-  <si>
     <t>EMSB_block</t>
   </si>
   <si>
@@ -267,12 +261,6 @@
     <t>SSPDG</t>
   </si>
   <si>
-    <t>STAI_likert_block</t>
-  </si>
-  <si>
-    <t>STAIY_likert_block</t>
-  </si>
-  <si>
     <t>ULS_likert_block</t>
   </si>
   <si>
@@ -280,6 +268,18 @@
   </si>
   <si>
     <t>Demographics_block</t>
+  </si>
+  <si>
+    <t>STAI-Y1</t>
+  </si>
+  <si>
+    <t>STAI-Y2</t>
+  </si>
+  <si>
+    <t>STAIY2_likert_block</t>
+  </si>
+  <si>
+    <t>STAIY1_likert_block</t>
   </si>
 </sst>
 </file>
@@ -324,7 +324,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -348,9 +348,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -388,7 +388,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -494,7 +494,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -636,7 +636,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -647,7 +647,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -660,13 +660,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -677,7 +677,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -688,18 +688,18 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -710,18 +710,18 @@
         <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -732,7 +732,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -743,7 +743,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -751,21 +751,21 @@
         <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -776,7 +776,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -787,18 +787,18 @@
         <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -806,10 +806,10 @@
         <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -828,7 +828,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -847,7 +847,7 @@
         <v>30</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -858,7 +858,7 @@
         <v>31</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -869,29 +869,29 @@
         <v>32</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -902,29 +902,29 @@
         <v>35</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -932,10 +932,10 @@
         <v>14</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -943,21 +943,21 @@
         <v>15</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>